<commit_message>
Added Phase 2 details to Chart
Added design document details and work splits
</commit_message>
<xml_diff>
--- a/Phase 2 Documents/CS401 Gantt Chart - Updated P2.xlsx
+++ b/Phase 2 Documents/CS401 Gantt Chart - Updated P2.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\communicationsGroup4\Phase 2 Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE43F6D-11C4-4AEA-BFC0-08380B08EF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Development</t>
   </si>
@@ -133,9 +142,6 @@
     <t>- 7. UML Sequence Diagrams</t>
   </si>
   <si>
-    <t>Grantt Chart</t>
-  </si>
-  <si>
     <t>Project Presentation Slides</t>
   </si>
   <si>
@@ -148,9 +154,6 @@
     <t>Phase 2</t>
   </si>
   <si>
-    <t>Design</t>
-  </si>
-  <si>
     <t>Implementation</t>
   </si>
   <si>
@@ -164,26 +167,70 @@
   </si>
   <si>
     <t>Final Presentation</t>
+  </si>
+  <si>
+    <t>Design Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a. IT Admin Diagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    b. GUI and Client Diagrams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a. Paper Prototype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    b. Mockup Prototype</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
+  </si>
+  <si>
+    <t>Phase Presentation</t>
+  </si>
+  <si>
+    <t>Talhah/Zoheb</t>
+  </si>
+  <si>
+    <t>1. Class Diagram Updated</t>
+  </si>
+  <si>
+    <t>2. Classes Descriptions</t>
+  </si>
+  <si>
+    <t>3. Sequence Diagrams</t>
+  </si>
+  <si>
+    <t>4. Prototype</t>
+  </si>
+  <si>
+    <t>Kenny/Talhah</t>
+  </si>
+  <si>
+    <t>Zoheb/Kenny/Talhah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -194,7 +241,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -209,8 +256,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
-    <border/>
+  <borders count="17">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF284E3F"/>
@@ -224,6 +277,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -238,6 +292,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -252,6 +307,7 @@
       <bottom style="thin">
         <color rgb="FF284E3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -266,6 +322,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -280,6 +337,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -294,34 +352,37 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF8F9FA"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF8F9FA"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -336,20 +397,22 @@
       <bottom style="thin">
         <color rgb="FFFF0000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFF8F9FA"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -364,6 +427,7 @@
       <bottom style="thin">
         <color rgb="FFF4CCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -378,193 +442,203 @@
       <bottom style="thin">
         <color rgb="FFFF0000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF8F9FA"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF8F9FA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF356854"/>
           <bgColor rgb="FF356854"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Sheet1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:N27" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N38">
   <tableColumns count="14">
-    <tableColumn name="Development" id="1"/>
-    <tableColumn name="Assigned to" id="2"/>
-    <tableColumn name="Week 5" id="3"/>
-    <tableColumn name="Week 6" id="4"/>
-    <tableColumn name="Week 7" id="5"/>
-    <tableColumn name="Week 8" id="6"/>
-    <tableColumn name="Week 9" id="7"/>
-    <tableColumn name="Week 10" id="8"/>
-    <tableColumn name="Week 11" id="9"/>
-    <tableColumn name="Week 12" id="10"/>
-    <tableColumn name="Week 13" id="11"/>
-    <tableColumn name="Week 14" id="12"/>
-    <tableColumn name="Week 15" id="13"/>
-    <tableColumn name="Week 16" id="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Development"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assigned to"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Week 5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Week 6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Week 7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Week 8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Week 9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Week 10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Week 11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Week 12"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Week 13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Week 14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Week 15"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Week 16"/>
   </tableColumns>
-  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -754,26 +828,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.25"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
@@ -857,13 +935,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="N3" s="10"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -872,203 +950,315 @@
       <c r="E4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="14" t="s">
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="14" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="N8" s="13"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="14" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
       <c r="N9" s="10"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="14" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
       <c r="N11" s="10"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="14" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="N13" s="10"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="18" t="s">
+      <c r="E14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15">
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="N15" s="10"/>
     </row>
-    <row r="16">
-      <c r="A16" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="20" t="s">
-        <v>45</v>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="N30" s="10"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="N18" s="13"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="20" t="s">
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9"/>
+      <c r="N32" s="10"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="N19" s="10"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
+      <c r="M33" s="11"/>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="N20" s="13"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="9"/>
-      <c r="N21" s="10"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="N23" s="21"/>
-    </row>
-    <row r="24">
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25">
-      <c r="N25" s="10"/>
-    </row>
-    <row r="26">
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="22"/>
-      <c r="N27" s="23"/>
+      <c r="N34" s="18"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="19"/>
+      <c r="N38" s="20"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>